<commit_message>
added dma location file
</commit_message>
<xml_diff>
--- a/Top 100 BEER with Owner.xlsx
+++ b/Top 100 BEER with Owner.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nflsz\Documents\Northwestern\Research\Merger\Mergers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2DF19B51-4C4B-4EB1-8882-5D22C57967E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A866DE48-82B7-4757-8282-35474CCB610B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Top 100 BEER" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -565,7 +576,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1399,11 +1410,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2764,7 +2775,7 @@
         <v>0</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" ref="F67:F130" si="1">D69</f>
+        <f t="shared" ref="F69:F130" si="1">D69</f>
         <v>Craft Brew Alliance</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed bug in adding features
</commit_message>
<xml_diff>
--- a/Top 100 BEER with Owner.xlsx
+++ b/Top 100 BEER with Owner.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nflsz\Documents\Northwestern\Research\Merger\Mergers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A866DE48-82B7-4757-8282-35474CCB610B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D4B68C-E473-4F21-85B9-72686B9A594B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Top 100 BEER" sheetId="1" r:id="rId1"/>
+    <sheet name="Owning Firms" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Top 100 BEER'!$D:$D</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="0">'Top 100 BEER'!$I$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="180">
   <si>
     <t>brand_code_uc</t>
   </si>
@@ -1411,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F145"/>
+  <dimension ref="A1:I145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1425,7 +1429,7 @@
     <col min="6" max="6" width="22.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1441,8 +1445,11 @@
       <c r="F1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1462,8 +1469,11 @@
         <f>D2</f>
         <v>Diageo</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1483,8 +1493,11 @@
         <f t="shared" ref="F3:F66" si="0">D3</f>
         <v>Diageo</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1504,8 +1517,11 @@
         <f t="shared" si="0"/>
         <v>Molson Coors</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1525,8 +1541,11 @@
         <f t="shared" si="0"/>
         <v>Molson Coors</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1537,17 +1556,19 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6">
+        <v>2008</v>
+      </c>
+      <c r="F6" t="s">
         <v>148</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>AB InBev</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1561,13 +1582,16 @@
         <v>171</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F7" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1581,13 +1605,16 @@
         <v>171</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F8" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1601,13 +1628,16 @@
         <v>171</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F9" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1621,13 +1651,16 @@
         <v>171</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F10" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1641,13 +1674,16 @@
         <v>171</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F11" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1661,13 +1697,16 @@
         <v>171</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F12" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1687,8 +1726,11 @@
         <f t="shared" si="0"/>
         <v>Yuengling</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1702,13 +1744,13 @@
         <v>171</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F14" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1722,13 +1764,16 @@
         <v>171</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>2008</v>
       </c>
       <c r="F15" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1748,8 +1793,11 @@
         <f t="shared" si="0"/>
         <v>Yuengling</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1769,8 +1817,11 @@
         <f t="shared" si="0"/>
         <v>Yuengling</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1790,8 +1841,11 @@
         <f t="shared" si="0"/>
         <v>Genesee</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1805,13 +1859,16 @@
         <v>171</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F19" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1825,13 +1882,16 @@
         <v>171</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F20" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I20" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1845,13 +1905,16 @@
         <v>156</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F21" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1870,8 +1933,11 @@
       <c r="F22" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1890,8 +1956,11 @@
       <c r="F23" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1911,8 +1980,11 @@
         <f t="shared" si="0"/>
         <v>Moosehead</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I24" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1931,8 +2003,11 @@
       <c r="F25" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1946,14 +2021,17 @@
         <v>152</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
         <v>Goya Foods</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1972,8 +2050,11 @@
       <c r="F27" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1993,8 +2074,11 @@
         <f t="shared" si="0"/>
         <v>Pyramid Breweries</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2014,8 +2098,11 @@
         <f t="shared" si="0"/>
         <v>Pyramid Breweries</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2035,8 +2122,11 @@
         <f t="shared" si="0"/>
         <v>Gambrinus</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I30" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2050,13 +2140,16 @@
         <v>171</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F31" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I31" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2070,10 +2163,13 @@
         <v>171</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F32" t="s">
         <v>148</v>
+      </c>
+      <c r="I32" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -2090,7 +2186,7 @@
         <v>171</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F33" t="s">
         <v>148</v>
@@ -2110,7 +2206,7 @@
         <v>156</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F34" t="s">
         <v>177</v>
@@ -2151,7 +2247,7 @@
         <v>171</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F36" t="s">
         <v>148</v>
@@ -2171,7 +2267,7 @@
         <v>171</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F37" t="s">
         <v>148</v>
@@ -2191,7 +2287,7 @@
         <v>171</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F38" t="s">
         <v>148</v>
@@ -2211,7 +2307,7 @@
         <v>156</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F39" t="s">
         <v>177</v>
@@ -2231,7 +2327,7 @@
         <v>171</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F40" t="s">
         <v>148</v>
@@ -2293,7 +2389,7 @@
         <v>156</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F43" t="s">
         <v>177</v>
@@ -2327,6 +2423,9 @@
       <c r="D45" t="s">
         <v>156</v>
       </c>
+      <c r="E45">
+        <v>2008</v>
+      </c>
       <c r="F45" t="s">
         <v>177</v>
       </c>
@@ -2362,6 +2461,9 @@
       <c r="D47" t="s">
         <v>147</v>
       </c>
+      <c r="E47">
+        <v>2008</v>
+      </c>
       <c r="F47" t="s">
         <v>177</v>
       </c>
@@ -2380,7 +2482,7 @@
         <v>171</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F48" t="s">
         <v>148</v>
@@ -2436,7 +2538,7 @@
         <v>171</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F51" t="s">
         <v>148</v>
@@ -2456,7 +2558,7 @@
         <v>171</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F52" t="s">
         <v>148</v>
@@ -2476,7 +2578,7 @@
         <v>171</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F53" t="s">
         <v>148</v>
@@ -2516,6 +2618,9 @@
       <c r="D55" t="s">
         <v>168</v>
       </c>
+      <c r="E55">
+        <v>2008</v>
+      </c>
       <c r="F55" t="s">
         <v>156</v>
       </c>
@@ -2533,6 +2638,9 @@
       <c r="D56" t="s">
         <v>169</v>
       </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
         <v>CTL Beer</v>
@@ -2552,7 +2660,7 @@
         <v>171</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F57" t="s">
         <v>148</v>
@@ -2572,7 +2680,7 @@
         <v>171</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F58" t="s">
         <v>148</v>
@@ -2592,7 +2700,7 @@
         <v>171</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F59" t="s">
         <v>148</v>
@@ -2612,7 +2720,7 @@
         <v>171</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F60" t="s">
         <v>148</v>
@@ -2667,6 +2775,9 @@
       <c r="D63" t="s">
         <v>156</v>
       </c>
+      <c r="E63">
+        <v>2008</v>
+      </c>
       <c r="F63" t="s">
         <v>177</v>
       </c>
@@ -2684,6 +2795,9 @@
       <c r="D64" t="s">
         <v>156</v>
       </c>
+      <c r="E64">
+        <v>2008</v>
+      </c>
       <c r="F64" t="s">
         <v>177</v>
       </c>
@@ -2737,6 +2851,9 @@
       <c r="D67" t="s">
         <v>156</v>
       </c>
+      <c r="E67">
+        <v>2008</v>
+      </c>
       <c r="F67" t="s">
         <v>177</v>
       </c>
@@ -2754,6 +2871,9 @@
       <c r="D68" t="s">
         <v>171</v>
       </c>
+      <c r="E68">
+        <v>2008</v>
+      </c>
       <c r="F68" t="s">
         <v>148</v>
       </c>
@@ -2813,6 +2933,9 @@
       <c r="D71" t="s">
         <v>170</v>
       </c>
+      <c r="E71">
+        <v>2008</v>
+      </c>
       <c r="F71" t="s">
         <v>148</v>
       </c>
@@ -2902,6 +3025,9 @@
       <c r="D76" t="s">
         <v>171</v>
       </c>
+      <c r="E76">
+        <v>2008</v>
+      </c>
       <c r="F76" t="s">
         <v>148</v>
       </c>
@@ -2956,7 +3082,7 @@
         <v>170</v>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F79" t="s">
         <v>148</v>
@@ -2975,6 +3101,9 @@
       <c r="D80" t="s">
         <v>171</v>
       </c>
+      <c r="E80">
+        <v>2008</v>
+      </c>
       <c r="F80" t="s">
         <v>148</v>
       </c>
@@ -2993,7 +3122,7 @@
         <v>156</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F81" t="s">
         <v>177</v>
@@ -3012,6 +3141,9 @@
       <c r="D82" t="s">
         <v>171</v>
       </c>
+      <c r="E82">
+        <v>2008</v>
+      </c>
       <c r="F82" t="s">
         <v>148</v>
       </c>
@@ -3030,7 +3162,7 @@
         <v>156</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F83" t="s">
         <v>177</v>
@@ -3049,6 +3181,9 @@
       <c r="D84" t="s">
         <v>171</v>
       </c>
+      <c r="E84">
+        <v>2008</v>
+      </c>
       <c r="F84" t="s">
         <v>148</v>
       </c>
@@ -3067,7 +3202,7 @@
         <v>156</v>
       </c>
       <c r="E85">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F85" t="s">
         <v>177</v>
@@ -3105,7 +3240,7 @@
         <v>156</v>
       </c>
       <c r="E87">
-        <v>1</v>
+        <v>2008</v>
       </c>
       <c r="F87" t="s">
         <v>177</v>
@@ -3160,6 +3295,9 @@
       <c r="D90" t="s">
         <v>156</v>
       </c>
+      <c r="E90">
+        <v>2008</v>
+      </c>
       <c r="F90" t="s">
         <v>177</v>
       </c>
@@ -3177,6 +3315,9 @@
       <c r="D91" t="s">
         <v>156</v>
       </c>
+      <c r="E91">
+        <v>2008</v>
+      </c>
       <c r="F91" t="s">
         <v>177</v>
       </c>
@@ -3194,6 +3335,9 @@
       <c r="D92" t="s">
         <v>156</v>
       </c>
+      <c r="E92">
+        <v>2008</v>
+      </c>
       <c r="F92" t="s">
         <v>177</v>
       </c>
@@ -3247,6 +3391,9 @@
       <c r="D95" t="s">
         <v>156</v>
       </c>
+      <c r="E95">
+        <v>2008</v>
+      </c>
       <c r="F95" t="s">
         <v>177</v>
       </c>
@@ -3444,6 +3591,9 @@
       <c r="D106" t="s">
         <v>147</v>
       </c>
+      <c r="E106">
+        <v>2008</v>
+      </c>
       <c r="F106" t="str">
         <f t="shared" si="1"/>
         <v>Molson Coors</v>
@@ -3462,6 +3612,9 @@
       <c r="D107" t="s">
         <v>170</v>
       </c>
+      <c r="E107">
+        <v>2008</v>
+      </c>
       <c r="F107" t="s">
         <v>148</v>
       </c>
@@ -3515,6 +3668,9 @@
       <c r="D110" t="s">
         <v>147</v>
       </c>
+      <c r="E110">
+        <v>2008</v>
+      </c>
       <c r="F110" t="s">
         <v>177</v>
       </c>
@@ -3532,6 +3688,9 @@
       <c r="D111" t="s">
         <v>147</v>
       </c>
+      <c r="E111">
+        <v>2008</v>
+      </c>
       <c r="F111" t="s">
         <v>177</v>
       </c>
@@ -3585,6 +3744,9 @@
       <c r="D114" t="s">
         <v>156</v>
       </c>
+      <c r="E114">
+        <v>2008</v>
+      </c>
       <c r="F114" t="s">
         <v>177</v>
       </c>
@@ -3602,6 +3764,9 @@
       <c r="D115" t="s">
         <v>156</v>
       </c>
+      <c r="E115">
+        <v>2008</v>
+      </c>
       <c r="F115" t="s">
         <v>177</v>
       </c>
@@ -3619,6 +3784,9 @@
       <c r="D116" t="s">
         <v>156</v>
       </c>
+      <c r="E116">
+        <v>2008</v>
+      </c>
       <c r="F116" t="s">
         <v>177</v>
       </c>
@@ -3654,6 +3822,9 @@
       <c r="D118" t="s">
         <v>156</v>
       </c>
+      <c r="E118">
+        <v>2008</v>
+      </c>
       <c r="F118" t="s">
         <v>177</v>
       </c>
@@ -3671,6 +3842,9 @@
       <c r="D119" t="s">
         <v>147</v>
       </c>
+      <c r="E119">
+        <v>2008</v>
+      </c>
       <c r="F119" t="s">
         <v>177</v>
       </c>
@@ -3688,6 +3862,9 @@
       <c r="D120" t="s">
         <v>147</v>
       </c>
+      <c r="E120">
+        <v>2008</v>
+      </c>
       <c r="F120" t="s">
         <v>177</v>
       </c>
@@ -3705,6 +3882,9 @@
       <c r="D121" t="s">
         <v>147</v>
       </c>
+      <c r="E121">
+        <v>2008</v>
+      </c>
       <c r="F121" t="s">
         <v>177</v>
       </c>
@@ -3758,6 +3938,9 @@
       <c r="D124" t="s">
         <v>147</v>
       </c>
+      <c r="E124">
+        <v>2008</v>
+      </c>
       <c r="F124" t="s">
         <v>177</v>
       </c>
@@ -3811,6 +3994,9 @@
       <c r="D127" t="s">
         <v>147</v>
       </c>
+      <c r="E127">
+        <v>2008</v>
+      </c>
       <c r="F127" t="s">
         <v>177</v>
       </c>
@@ -3900,6 +4086,9 @@
       <c r="D132" t="s">
         <v>170</v>
       </c>
+      <c r="E132">
+        <v>2008</v>
+      </c>
       <c r="F132" t="s">
         <v>148</v>
       </c>
@@ -3917,6 +4106,9 @@
       <c r="D133" t="s">
         <v>170</v>
       </c>
+      <c r="E133">
+        <v>2008</v>
+      </c>
       <c r="F133" t="s">
         <v>148</v>
       </c>
@@ -3952,6 +4144,9 @@
       <c r="D135" t="s">
         <v>170</v>
       </c>
+      <c r="E135">
+        <v>2008</v>
+      </c>
       <c r="F135" t="s">
         <v>148</v>
       </c>
@@ -3969,6 +4164,9 @@
       <c r="D136" t="s">
         <v>170</v>
       </c>
+      <c r="E136">
+        <v>2008</v>
+      </c>
       <c r="F136" t="s">
         <v>148</v>
       </c>
@@ -3986,6 +4184,9 @@
       <c r="D137" t="s">
         <v>156</v>
       </c>
+      <c r="E137">
+        <v>2008</v>
+      </c>
       <c r="F137" t="str">
         <f t="shared" si="2"/>
         <v>SABMiller</v>
@@ -4058,6 +4259,9 @@
       <c r="D141" t="s">
         <v>156</v>
       </c>
+      <c r="E141">
+        <v>2008</v>
+      </c>
       <c r="F141" t="s">
         <v>177</v>
       </c>
@@ -4137,4 +4341,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4199ACD-5F13-4077-881C-F67DDF7BE9FC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>